<commit_message>
LOOCV, new homo dna models
</commit_message>
<xml_diff>
--- a/data/scFv/scfv_lysis.xlsx
+++ b/data/scFv/scfv_lysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/florian_gisperg_tuwien_ac_at/Documents/01_Uni/01_PhD/05_Projects/HPH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/florian_gisperg_tuwien_ac_at/Documents/01_Uni/01_PhD/05_Projects/Homogenisation/data/scFv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="50" documentId="8_{9FCC5876-D8A6-413D-8318-F458C6FEB781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21D0E1B-12F0-4BAA-A6E4-7DFCA76D3386}"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K37"/>
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>